<commit_message>
Pridedu dar console apllicationa skelbimu parsinimui
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,13 +69,39 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,14 +113,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,7 +429,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,26 +456,26 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Standartinė tema nustatyta ir rašomas taskų listas
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Taskas</t>
   </si>
@@ -27,62 +27,23 @@
     <t>Artas</t>
   </si>
   <si>
-    <t>SVN public</t>
-  </si>
-  <si>
     <t>Ignas</t>
   </si>
   <si>
-    <t>Plugin, interface system</t>
-  </si>
-  <si>
-    <t>Saving DB error</t>
-  </si>
-  <si>
-    <t>Object cache in GenericDbHelper</t>
-  </si>
-  <si>
-    <t>Console service advert</t>
-  </si>
-  <si>
-    <t>Modulinė sistema, token-login atskirame modulyje</t>
-  </si>
-  <si>
-    <t>Db versijavimo sistema</t>
-  </si>
-  <si>
-    <t>Release deployment sistema</t>
-  </si>
-  <si>
-    <t>Perkelti modulius</t>
-  </si>
-  <si>
-    <t>Modulių testai</t>
-  </si>
-  <si>
-    <t>Web'o testai</t>
-  </si>
-  <si>
-    <t>Registracijos forma, username panaikinti ir palikti tik mail</t>
-  </si>
-  <si>
-    <t>Password restore forma</t>
-  </si>
-  <si>
-    <t>Dizainas</t>
-  </si>
-  <si>
-    <t>Pakurti serverį</t>
-  </si>
-  <si>
-    <t>Licencijų modulis</t>
+    <t>Autoscout24.de</t>
+  </si>
+  <si>
+    <t>Logas parserio</t>
+  </si>
+  <si>
+    <t>Edit disable settings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,26 +60,13 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="186"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,23 +78,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,131 +407,27 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pakoreguotas parseris, cache ir multi thread
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +524,13 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mini pakeitimai, senas solutionas metamas lauk.
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Taskas</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Perkelti serverį į kitą mašiną</t>
+  </si>
+  <si>
+    <t>Rūšiavimas skelbimų pagal radimo datą</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,13 +538,13 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -568,13 +571,13 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -631,6 +634,17 @@
       </c>
       <c r="C15" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mini pakeitimai, mėginta daryti auto refresh - nesigavo.
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>Taskas</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Rūšiavimas skelbimų pagal radimo datą</t>
+  </si>
+  <si>
+    <t>DB auto backups</t>
+  </si>
+  <si>
+    <t>Taisyklės</t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,6 +669,28 @@
         <v>3</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pakeitimai, mėginta daryti, kad veiktų open link normaliai
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Taskas</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Prisijungusių userių sąrašas</t>
+  </si>
+  <si>
+    <t>Naujų skelbimų garsas</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +726,17 @@
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Padarytas nuotraukų ir mailo siuntimas. Optimaizintas parseris.
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,13 +628,13 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kiekviename parseryje pridetas Paveiksliuku gavimas
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -512,9 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -788,13 +786,13 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Persikrauna (kas 1min) tik nauju skelbimu puslapis
</commit_message>
<xml_diff>
--- a/Docs/TODO.xlsx
+++ b/Docs/TODO.xlsx
@@ -555,13 +555,13 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>